<commit_message>
Tidy up to prepare for submission
Lots of files renamed
Backups deleted
Docs updated
</commit_message>
<xml_diff>
--- a/docs/analysis/Data Analysis 16.12.15.xlsx
+++ b/docs/analysis/Data Analysis 16.12.15.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\GitHub\researchProject\docs\analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="2"/>
+    <workbookView xWindow="390" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A - Steady State" sheetId="7" r:id="rId1"/>
     <sheet name="A - Step Change" sheetId="8" r:id="rId2"/>
     <sheet name="B - Steady State" sheetId="9" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -59,13 +64,24 @@
   <si>
     <t>Minimum Varience Controller - 60s</t>
   </si>
+  <si>
+    <t>Shifted data For graphs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,20 +109,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -126,11 +163,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -839,33 +879,47 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="87807872"/>
-        <c:axId val="87806336"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="389326720"/>
+        <c:axId val="390889056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="87807872"/>
+        <c:axId val="389326720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87806336"/>
+        <c:crossAx val="390889056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87806336"/>
+        <c:axId val="390889056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="430"/>
           <c:min val="330"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87807872"/>
+        <c:crossAx val="389326720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -873,8 +927,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -886,7 +943,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -934,7 +1001,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -949,6 +1018,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1421,31 +1491,45 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="138076160"/>
-        <c:axId val="138077696"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="338770560"/>
+        <c:axId val="342472096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="138076160"/>
+        <c:axId val="338770560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138077696"/>
+        <c:crossAx val="342472096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="138077696"/>
+        <c:axId val="342472096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="138076160"/>
+        <c:crossAx val="338770560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1453,8 +1537,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1466,7 +1553,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1478,25 +1575,31 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
+              <a:rPr lang="en-GB" sz="1400" b="0" baseline="0"/>
               <a:t>Graphical Plot of Controller Performance During a Setpoint Change</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB"/>
+            <a:endParaRPr lang="en-GB" sz="1400" b="0"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>PV</c:v>
+            <c:v>SP</c:v>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'A - Step Change'!$A$5:$A$68</c:f>
@@ -1700,213 +1803,207 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'A - Step Change'!$B$5:$B$68</c:f>
+              <c:f>'A - Step Change'!$I$5:$I$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="64"/>
                 <c:pt idx="0">
-                  <c:v>396</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>399</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>407</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>404</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>406</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>392</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>393</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>396</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>408</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>376</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>380</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>387</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>397</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>403</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>407</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>412</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>410</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>397</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>394</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>393</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>389</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>402</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>384</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>380</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>384</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>386</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>392</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>396</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>394</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>399</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>409</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>410</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>411</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>413</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>411</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>420</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>420</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>437</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>446</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>451</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>476</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>488</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>503</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>523</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>545</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>560</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>578</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>595</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>599</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>612</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>598</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>596</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>574</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>559</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>518</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>487</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>447</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>420</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>394</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>369</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>334</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>273</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>294</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="2"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>SP</c:v>
+            <c:v>OP</c:v>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'A - Step Change'!$A$5:$A$68</c:f>
@@ -2110,213 +2207,207 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'A - Step Change'!$C$5:$C$68</c:f>
+              <c:f>'A - Step Change'!$J$5:$J$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="64"/>
                 <c:pt idx="0">
-                  <c:v>400</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>400</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>37.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>400</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>400</c:v>
+                  <c:v>36.6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>400</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>400</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>400</c:v>
+                  <c:v>38.1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>400</c:v>
+                  <c:v>35.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>400</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>400</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>400</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>400</c:v>
+                  <c:v>39.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>400</c:v>
+                  <c:v>37.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>38.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>400</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>400</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>400</c:v>
+                  <c:v>36.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>400</c:v>
+                  <c:v>37.9</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>400</c:v>
+                  <c:v>37.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>400</c:v>
+                  <c:v>38.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>400</c:v>
+                  <c:v>35.9</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>400</c:v>
+                  <c:v>37.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>400</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>400</c:v>
+                  <c:v>38.1</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>400</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>400</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>400</c:v>
+                  <c:v>37.1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>400</c:v>
+                  <c:v>38.6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>400</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>400</c:v>
+                  <c:v>39.1</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>400</c:v>
+                  <c:v>37.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>400</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>400</c:v>
+                  <c:v>36.9</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>500</c:v>
+                  <c:v>39.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>500</c:v>
+                  <c:v>38.9</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>500</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>500</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>500</c:v>
+                  <c:v>41.2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>500</c:v>
+                  <c:v>41.7</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>500</c:v>
+                  <c:v>43.4</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>500</c:v>
+                  <c:v>42.7</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>500</c:v>
+                  <c:v>44.4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>500</c:v>
+                  <c:v>43.6</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>500</c:v>
+                  <c:v>45.1</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>500</c:v>
+                  <c:v>43.1</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>500</c:v>
+                  <c:v>44.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>500</c:v>
+                  <c:v>41.3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>500</c:v>
+                  <c:v>42.1</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>38.1</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>500</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>500</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>500</c:v>
+                  <c:v>35.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>500</c:v>
+                  <c:v>31.9</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>500</c:v>
+                  <c:v>33.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>500</c:v>
+                  <c:v>31.4</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>500</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>500</c:v>
+                  <c:v>32.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>500</c:v>
+                  <c:v>33.4</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>500</c:v>
+                  <c:v>32.700000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="0"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Valve OP</c:v>
+            <c:v>PV</c:v>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'A - Step Change'!$A$5:$A$68</c:f>
@@ -2520,234 +2611,283 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'A - Step Change'!$D$5:$D$68</c:f>
+              <c:f>'A - Step Change'!$H$5:$H$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="64"/>
                 <c:pt idx="0">
-                  <c:v>375</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>378</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>376</c:v>
+                  <c:v>40.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>373</c:v>
+                  <c:v>40.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>372</c:v>
+                  <c:v>40.6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>366</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>375</c:v>
+                  <c:v>39.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>372</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>381</c:v>
+                  <c:v>40.799999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>352</c:v>
+                  <c:v>37.6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>378</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>387</c:v>
+                  <c:v>38.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>387</c:v>
+                  <c:v>39.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>393</c:v>
+                  <c:v>40.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>378</c:v>
+                  <c:v>40.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>388</c:v>
+                  <c:v>41.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>350</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>376</c:v>
+                  <c:v>39.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>365</c:v>
+                  <c:v>39.4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>379</c:v>
+                  <c:v>39.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>373</c:v>
+                  <c:v>38.9</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>382</c:v>
+                  <c:v>40.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>359</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>375</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>372</c:v>
+                  <c:v>38.4</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>381</c:v>
+                  <c:v>38.6</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>376</c:v>
+                  <c:v>39.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>387</c:v>
+                  <c:v>39.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>371</c:v>
+                  <c:v>39.4</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>386</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>376</c:v>
+                  <c:v>40.9</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>391</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>372</c:v>
+                  <c:v>41.1</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>396</c:v>
+                  <c:v>41.3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>369</c:v>
+                  <c:v>41.1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>395</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>389</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>400</c:v>
+                  <c:v>43.7</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>408</c:v>
+                  <c:v>44.6</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>412</c:v>
+                  <c:v>45.1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>417</c:v>
+                  <c:v>47.6</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>434</c:v>
+                  <c:v>48.8</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>427</c:v>
+                  <c:v>50.3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>444</c:v>
+                  <c:v>52.3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>436</c:v>
+                  <c:v>54.5</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>451</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>431</c:v>
+                  <c:v>57.8</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>445</c:v>
+                  <c:v>59.5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>413</c:v>
+                  <c:v>59.9</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>421</c:v>
+                  <c:v>61.2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>381</c:v>
+                  <c:v>59.8</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>385</c:v>
+                  <c:v>59.6</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>345</c:v>
+                  <c:v>57.4</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>352</c:v>
+                  <c:v>55.9</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>319</c:v>
+                  <c:v>51.8</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>332</c:v>
+                  <c:v>48.7</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>314</c:v>
+                  <c:v>44.7</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>330</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>323</c:v>
+                  <c:v>39.4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>334</c:v>
+                  <c:v>36.9</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>327</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>413</c:v>
+                  <c:v>33.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="135393280"/>
-        <c:axId val="135394816"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395401888"/>
+        <c:axId val="395402448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135393280"/>
+        <c:axId val="395401888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135394816"/>
+        <c:crossAx val="395402448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="135394816"/>
+        <c:axId val="395402448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0"/>
+                  <a:t>PV,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0" baseline="0"/>
+                  <a:t> SP, OP (%)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" b="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135393280"/>
+        <c:crossAx val="395401888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2755,8 +2895,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2768,7 +2911,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2780,59 +2933,55 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
+              <a:rPr lang="en-GB" b="0" baseline="0"/>
               <a:t>Variation in </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="el-GR" baseline="0">
+              <a:rPr lang="el-GR" b="0" baseline="0">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
               <a:t>α</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0">
+              <a:rPr lang="en-GB" b="0" baseline="0">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
               <a:t> &amp; </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="el-GR" baseline="0">
+              <a:rPr lang="el-GR" b="0" baseline="0">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
               <a:t>β</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0">
+              <a:rPr lang="en-GB" b="0" baseline="0">
                 <a:latin typeface="Calibri"/>
               </a:rPr>
-              <a:t> During a Setpoint Change</a:t>
+              <a:t> during a setpoint change</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB"/>
+            <a:endParaRPr lang="en-GB" b="0"/>
           </a:p>
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="4.649149903193512E-2"/>
-          <c:y val="0.12693079654635936"/>
-          <c:w val="0.81810074521934761"/>
-          <c:h val="0.8395774396978658"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>α</c:v>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'A - Step Change'!$A$5:$A$68</c:f>
@@ -3223,19 +3372,10 @@
                 <c:pt idx="60">
                   <c:v>-11.283862444842734</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>-37.756959123975086</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>-1.0033046144804771</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>-0.89970008462353257</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3243,6 +3383,9 @@
           <c:tx>
             <c:v>β</c:v>
           </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:xVal>
             <c:numRef>
               <c:f>'A - Step Change'!$A$5:$A$68</c:f>
@@ -3633,47 +3776,103 @@
                 <c:pt idx="60">
                   <c:v>13.475645198133495</c:v>
                 </c:pt>
-                <c:pt idx="61">
-                  <c:v>39.435644885762571</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1.8707464851816269</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1.7692950143958737</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="137881472"/>
-        <c:axId val="137883008"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395405808"/>
+        <c:axId val="395406368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="137881472"/>
+        <c:axId val="395405808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2000"/>
           <c:min val="0"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0"/>
+                  <a:t>Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137883008"/>
+        <c:crossAx val="395406368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="137883008"/>
+        <c:axId val="395406368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="el-GR" b="0"/>
+                  <a:t>α</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0"/>
+                  <a:t>, </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="el-GR" b="0">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>β</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB" b="0"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137881472"/>
+        <c:crossAx val="395405808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3681,8 +3880,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3694,7 +3896,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3714,11 +3926,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4193,31 +4408,45 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="152061056"/>
-        <c:axId val="151377024"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395413088"/>
+        <c:axId val="395413648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="152061056"/>
+        <c:axId val="395413088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151377024"/>
+        <c:crossAx val="395413648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151377024"/>
+        <c:axId val="395413648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152061056"/>
+        <c:crossAx val="395413088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4225,8 +4454,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4238,7 +4470,17 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4286,7 +4528,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -4301,6 +4545,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4617,31 +4862,45 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="151418368"/>
-        <c:axId val="151419904"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="395823840"/>
+        <c:axId val="395824400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="151418368"/>
+        <c:axId val="395823840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151419904"/>
+        <c:crossAx val="395824400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="151419904"/>
+        <c:axId val="395824400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151418368"/>
+        <c:crossAx val="395823840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4649,8 +4908,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4729,13 +4991,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>609599</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -4759,13 +5021,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -4789,16 +5051,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>71399</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4807,8 +5069,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8305800" y="1104899"/>
-          <a:ext cx="0" cy="3348000"/>
+          <a:off x="11601450" y="1114424"/>
+          <a:ext cx="0" cy="3076576"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4833,16 +5095,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>70425</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4851,8 +5113,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8305800" y="5495925"/>
-          <a:ext cx="0" cy="3528000"/>
+          <a:off x="11601450" y="5476875"/>
+          <a:ext cx="0" cy="3343275"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -4986,7 +5248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5018,9 +5280,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5052,6 +5315,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -5227,16 +5491,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -5244,7 +5508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5252,7 +5516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -5272,7 +5536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -5292,7 +5556,7 @@
         <v>1.5799999998999181</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>55</v>
       </c>
@@ -5312,7 +5576,7 @@
         <v>1.425540316351976</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>85</v>
       </c>
@@ -5332,7 +5596,7 @@
         <v>1.1838502131641466</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>115</v>
       </c>
@@ -5352,7 +5616,7 @@
         <v>1.1477589332296969</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>145</v>
       </c>
@@ -5372,7 +5636,7 @@
         <v>0.97003035306284258</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>175</v>
       </c>
@@ -5392,7 +5656,7 @@
         <v>1.3300395779221978</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>205</v>
       </c>
@@ -5412,7 +5676,7 @@
         <v>1.1217224091387747</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>235</v>
       </c>
@@ -5432,7 +5696,7 @@
         <v>1.6777689594630243</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>265</v>
       </c>
@@ -5452,7 +5716,7 @@
         <v>0.61308297541568346</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>295</v>
       </c>
@@ -5472,7 +5736,7 @@
         <v>1.9282791999604332</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>325</v>
       </c>
@@ -5492,7 +5756,7 @@
         <v>0.56252874082880822</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>355</v>
       </c>
@@ -5512,7 +5776,7 @@
         <v>2.3935132558498999</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>385</v>
       </c>
@@ -5532,7 +5796,7 @@
         <v>2.0849240041736672</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>415</v>
       </c>
@@ -5552,7 +5816,7 @@
         <v>0.70561003269295264</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>445</v>
       </c>
@@ -5572,7 +5836,7 @@
         <v>1.2558200537584971</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>475</v>
       </c>
@@ -5592,7 +5856,7 @@
         <v>0.50931706944890709</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>505</v>
       </c>
@@ -5612,7 +5876,7 @@
         <v>0.92318243386448129</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>535</v>
       </c>
@@ -5632,7 +5896,7 @@
         <v>0.58230096055256064</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>565</v>
       </c>
@@ -5652,7 +5916,7 @@
         <v>1.118693316420587</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>595</v>
       </c>
@@ -5672,7 +5936,7 @@
         <v>0.83512653961641803</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>625</v>
       </c>
@@ -5692,7 +5956,7 @@
         <v>2.2753431740172312</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>655</v>
       </c>
@@ -5712,7 +5976,7 @@
         <v>0.76011118845308845</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>685</v>
       </c>
@@ -5732,7 +5996,7 @@
         <v>1.8614994726074827</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>715</v>
       </c>
@@ -5752,7 +6016,7 @@
         <v>1.4356125020293851</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>745</v>
       </c>
@@ -5772,7 +6036,7 @@
         <v>6.5286421404409838</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>775</v>
       </c>
@@ -5792,7 +6056,7 @@
         <v>2.5368843004757786</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>805</v>
       </c>
@@ -5812,7 +6076,7 @@
         <v>7.651253724371978</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>835</v>
       </c>
@@ -5832,7 +6096,7 @@
         <v>1.8813366947840402</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>865</v>
       </c>
@@ -5852,7 +6116,7 @@
         <v>6.9815102813635832</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>895</v>
       </c>
@@ -5872,7 +6136,7 @@
         <v>2.889954736456235</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>925</v>
       </c>
@@ -5892,7 +6156,7 @@
         <v>4.566164987038154</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>955</v>
       </c>
@@ -5912,7 +6176,7 @@
         <v>2.2402203361596449</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>985</v>
       </c>
@@ -5932,7 +6196,7 @@
         <v>6.535040812517785</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1015</v>
       </c>
@@ -5952,7 +6216,7 @@
         <v>2.8305186305976546</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1045</v>
       </c>
@@ -5972,7 +6236,7 @@
         <v>12.210123063041202</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1075</v>
       </c>
@@ -5992,7 +6256,7 @@
         <v>5.9638951364371495</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1105</v>
       </c>
@@ -6012,7 +6276,7 @@
         <v>13.564367869556259</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1135</v>
       </c>
@@ -6032,7 +6296,7 @@
         <v>11.469047108336703</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1165</v>
       </c>
@@ -6052,7 +6316,7 @@
         <v>9.7761826836454517</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1195</v>
       </c>
@@ -6072,7 +6336,7 @@
         <v>9.7982631851010851</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1225</v>
       </c>
@@ -6092,7 +6356,7 @@
         <v>8.9483385609976001</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1255</v>
       </c>
@@ -6112,7 +6376,7 @@
         <v>6.8399750095594438</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1285</v>
       </c>
@@ -6132,7 +6396,7 @@
         <v>7.7682423748914022</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1315</v>
       </c>
@@ -6152,7 +6416,7 @@
         <v>5.8896749874611656</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1345</v>
       </c>
@@ -6172,7 +6436,7 @@
         <v>5.8698957849473841</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1375</v>
       </c>
@@ -6192,7 +6456,7 @@
         <v>4.6324542304230594</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1405</v>
       </c>
@@ -6212,7 +6476,7 @@
         <v>4.7467128124857112</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1435</v>
       </c>
@@ -6232,7 +6496,7 @@
         <v>3.7252824423653479</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1465</v>
       </c>
@@ -6252,7 +6516,7 @@
         <v>3.8580929203613987</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1495</v>
       </c>
@@ -6272,7 +6536,7 @@
         <v>3.1315385433364153</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1525</v>
       </c>
@@ -6292,7 +6556,7 @@
         <v>3.2669537843462546</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1555</v>
       </c>
@@ -6312,7 +6576,7 @@
         <v>2.7829610187852465</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1585</v>
       </c>
@@ -6332,7 +6596,7 @@
         <v>2.9569401050028916</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1615</v>
       </c>
@@ -6352,7 +6616,7 @@
         <v>2.6143375253653782</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1645</v>
       </c>
@@ -6372,7 +6636,7 @@
         <v>2.9625689716277508</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1675</v>
       </c>
@@ -6392,7 +6656,7 @@
         <v>2.827675851825346</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1705</v>
       </c>
@@ -6412,7 +6676,7 @@
         <v>3.5261935473191328</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1735</v>
       </c>
@@ -6432,7 +6696,7 @@
         <v>3.6881319756705038</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1765</v>
       </c>
@@ -6452,7 +6716,7 @@
         <v>5.2718229016720519</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1795</v>
       </c>
@@ -6472,7 +6736,7 @@
         <v>6.1772757572614383</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1825</v>
       </c>
@@ -6492,7 +6756,7 @@
         <v>13.475645198133495</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1855</v>
       </c>
@@ -6512,7 +6776,7 @@
         <v>39.435644885762571</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1885</v>
       </c>
@@ -6532,7 +6796,7 @@
         <v>1.8707464851816269</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1915</v>
       </c>
@@ -6559,16 +6823,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -6576,7 +6840,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -6584,7 +6848,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -6603,8 +6874,17 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -6623,8 +6903,20 @@
       <c r="F5">
         <v>1.5799999998999181</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5">
+        <f>B5/10</f>
+        <v>39.6</v>
+      </c>
+      <c r="I5">
+        <f>C5/10</f>
+        <v>40</v>
+      </c>
+      <c r="J5">
+        <f>D5/10</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>55</v>
       </c>
@@ -6643,8 +6935,20 @@
       <c r="F6">
         <v>1.425540316351976</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6">
+        <f t="shared" ref="H6:H68" si="0">B6/10</f>
+        <v>39.9</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ref="I6:I68" si="1">C6/10</f>
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J68" si="2">D6/10</f>
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>85</v>
       </c>
@@ -6663,8 +6967,20 @@
       <c r="F7">
         <v>1.1838502131641466</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>40.700000000000003</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>115</v>
       </c>
@@ -6683,8 +6999,20 @@
       <c r="F8">
         <v>1.1477589332296969</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>40.4</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>145</v>
       </c>
@@ -6703,8 +7031,20 @@
       <c r="F9">
         <v>0.97003035306284258</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>40.6</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>175</v>
       </c>
@@ -6723,8 +7063,20 @@
       <c r="F10">
         <v>1.3300395779221978</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>36.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>205</v>
       </c>
@@ -6743,8 +7095,20 @@
       <c r="F11">
         <v>1.1217224091387747</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>235</v>
       </c>
@@ -6763,8 +7127,20 @@
       <c r="F12">
         <v>1.6777689594630243</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>39.6</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>265</v>
       </c>
@@ -6783,8 +7159,20 @@
       <c r="F13">
         <v>0.61308297541568346</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>40.799999999999997</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>295</v>
       </c>
@@ -6803,8 +7191,20 @@
       <c r="F14">
         <v>1.9282791999604332</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>37.6</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>325</v>
       </c>
@@ -6823,8 +7223,20 @@
       <c r="F15">
         <v>0.56252874082880822</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>355</v>
       </c>
@@ -6843,8 +7255,20 @@
       <c r="F16">
         <v>2.3935132558498999</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>38.700000000000003</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>38.700000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>385</v>
       </c>
@@ -6863,8 +7287,20 @@
       <c r="F17">
         <v>2.0849240041736672</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>39.700000000000003</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>38.700000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>415</v>
       </c>
@@ -6883,8 +7319,20 @@
       <c r="F18">
         <v>0.70561003269295264</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>40.299999999999997</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>39.299999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>445</v>
       </c>
@@ -6903,8 +7351,20 @@
       <c r="F19">
         <v>1.2558200537584971</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>40.700000000000003</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>475</v>
       </c>
@@ -6923,8 +7383,20 @@
       <c r="F20">
         <v>0.50931706944890709</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>41.2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>38.799999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>505</v>
       </c>
@@ -6943,8 +7415,20 @@
       <c r="F21">
         <v>0.92318243386448129</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>535</v>
       </c>
@@ -6963,8 +7447,20 @@
       <c r="F22">
         <v>0.58230096055256064</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>39.700000000000003</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>565</v>
       </c>
@@ -6983,8 +7479,20 @@
       <c r="F23">
         <v>1.118693316420587</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>39.4</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>595</v>
       </c>
@@ -7003,8 +7511,20 @@
       <c r="F24">
         <v>0.83512653961641803</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>39.299999999999997</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>37.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>625</v>
       </c>
@@ -7023,8 +7543,20 @@
       <c r="F25">
         <v>2.2753431740172312</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>38.9</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>37.299999999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>655</v>
       </c>
@@ -7043,8 +7575,20 @@
       <c r="F26">
         <v>0.76011118845308845</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>40.200000000000003</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>685</v>
       </c>
@@ -7063,8 +7607,20 @@
       <c r="F27">
         <v>1.8614994726074827</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>38.4</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>715</v>
       </c>
@@ -7083,8 +7639,20 @@
       <c r="F28">
         <v>1.4356125020293851</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>745</v>
       </c>
@@ -7103,8 +7671,20 @@
       <c r="F29">
         <v>6.5286421404409838</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>38.4</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>775</v>
       </c>
@@ -7123,8 +7703,20 @@
       <c r="F30">
         <v>2.5368843004757786</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>38.6</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>805</v>
       </c>
@@ -7143,8 +7735,20 @@
       <c r="F31">
         <v>7.651253724371978</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>39.200000000000003</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>835</v>
       </c>
@@ -7163,8 +7767,20 @@
       <c r="F32">
         <v>1.8813366947840402</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>39.6</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>38.700000000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>865</v>
       </c>
@@ -7183,8 +7799,20 @@
       <c r="F33">
         <v>6.9815102813635832</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>39.4</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>37.1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>895</v>
       </c>
@@ -7203,8 +7831,20 @@
       <c r="F34">
         <v>2.889954736456235</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>39.9</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>38.6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>925</v>
       </c>
@@ -7223,8 +7863,20 @@
       <c r="F35">
         <v>4.566164987038154</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>40.9</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>955</v>
       </c>
@@ -7243,8 +7895,20 @@
       <c r="F36">
         <v>2.2402203361596449</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>985</v>
       </c>
@@ -7263,8 +7927,20 @@
       <c r="F37">
         <v>6.535040812517785</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>41.1</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>37.200000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1015</v>
       </c>
@@ -7283,8 +7959,20 @@
       <c r="F38">
         <v>2.8305186305976546</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>41.3</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>39.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1045</v>
       </c>
@@ -7303,8 +7991,20 @@
       <c r="F39">
         <v>12.210123063041202</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>41.1</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1075</v>
       </c>
@@ -7323,8 +8023,20 @@
       <c r="F40">
         <v>5.9638951364371495</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="2"/>
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1105</v>
       </c>
@@ -7343,8 +8055,20 @@
       <c r="F41">
         <v>13.564367869556259</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="2"/>
+        <v>38.9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1135</v>
       </c>
@@ -7363,8 +8087,20 @@
       <c r="F42">
         <v>11.469047108336703</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>43.7</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1165</v>
       </c>
@@ -7383,8 +8119,20 @@
       <c r="F43">
         <v>9.7761826836454517</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>44.6</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="2"/>
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1195</v>
       </c>
@@ -7403,8 +8151,20 @@
       <c r="F44">
         <v>9.7982631851010851</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>45.1</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="2"/>
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1225</v>
       </c>
@@ -7423,8 +8183,20 @@
       <c r="F45">
         <v>8.9483385609976001</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>47.6</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="2"/>
+        <v>41.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1255</v>
       </c>
@@ -7443,8 +8215,20 @@
       <c r="F46">
         <v>6.8399750095594438</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>48.8</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="2"/>
+        <v>43.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1285</v>
       </c>
@@ -7463,8 +8247,20 @@
       <c r="F47">
         <v>7.7682423748914022</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>50.3</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="2"/>
+        <v>42.7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1315</v>
       </c>
@@ -7483,8 +8279,20 @@
       <c r="F48">
         <v>5.8896749874611656</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>52.3</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="2"/>
+        <v>44.4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1345</v>
       </c>
@@ -7503,8 +8311,20 @@
       <c r="F49">
         <v>5.8698957849473841</v>
       </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="2"/>
+        <v>43.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1375</v>
       </c>
@@ -7523,8 +8343,20 @@
       <c r="F50">
         <v>4.6324542304230594</v>
       </c>
-    </row>
-    <row r="51" spans="1:6">
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="2"/>
+        <v>45.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1405</v>
       </c>
@@ -7543,8 +8375,20 @@
       <c r="F51">
         <v>4.7467128124857112</v>
       </c>
-    </row>
-    <row r="52" spans="1:6">
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>57.8</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="2"/>
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1435</v>
       </c>
@@ -7563,8 +8407,20 @@
       <c r="F52">
         <v>3.7252824423653479</v>
       </c>
-    </row>
-    <row r="53" spans="1:6">
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>59.5</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>44.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1465</v>
       </c>
@@ -7583,8 +8439,20 @@
       <c r="F53">
         <v>3.8580929203613987</v>
       </c>
-    </row>
-    <row r="54" spans="1:6">
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>59.9</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="2"/>
+        <v>41.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1495</v>
       </c>
@@ -7603,8 +8471,20 @@
       <c r="F54">
         <v>3.1315385433364153</v>
       </c>
-    </row>
-    <row r="55" spans="1:6">
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>61.2</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="2"/>
+        <v>42.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1525</v>
       </c>
@@ -7623,8 +8503,20 @@
       <c r="F55">
         <v>3.2669537843462546</v>
       </c>
-    </row>
-    <row r="56" spans="1:6">
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>59.8</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="2"/>
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1555</v>
       </c>
@@ -7643,8 +8535,20 @@
       <c r="F56">
         <v>2.7829610187852465</v>
       </c>
-    </row>
-    <row r="57" spans="1:6">
+      <c r="H56">
+        <f t="shared" si="0"/>
+        <v>59.6</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="2"/>
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1585</v>
       </c>
@@ -7663,8 +8567,20 @@
       <c r="F57">
         <v>2.9569401050028916</v>
       </c>
-    </row>
-    <row r="58" spans="1:6">
+      <c r="H57">
+        <f t="shared" si="0"/>
+        <v>57.4</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="2"/>
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1615</v>
       </c>
@@ -7683,8 +8599,20 @@
       <c r="F58">
         <v>2.6143375253653782</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="H58">
+        <f t="shared" si="0"/>
+        <v>55.9</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="2"/>
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1645</v>
       </c>
@@ -7703,8 +8631,20 @@
       <c r="F59">
         <v>2.9625689716277508</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="H59">
+        <f t="shared" si="0"/>
+        <v>51.8</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="2"/>
+        <v>31.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1675</v>
       </c>
@@ -7723,8 +8663,20 @@
       <c r="F60">
         <v>2.827675851825346</v>
       </c>
-    </row>
-    <row r="61" spans="1:6">
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>48.7</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="2"/>
+        <v>33.200000000000003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1705</v>
       </c>
@@ -7743,8 +8695,20 @@
       <c r="F61">
         <v>3.5261935473191328</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>44.7</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="2"/>
+        <v>31.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1735</v>
       </c>
@@ -7763,8 +8727,20 @@
       <c r="F62">
         <v>3.6881319756705038</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="H62">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1765</v>
       </c>
@@ -7783,8 +8759,20 @@
       <c r="F63">
         <v>5.2718229016720519</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
+      <c r="H63">
+        <f t="shared" si="0"/>
+        <v>39.4</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="2"/>
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1795</v>
       </c>
@@ -7803,8 +8791,20 @@
       <c r="F64">
         <v>6.1772757572614383</v>
       </c>
-    </row>
-    <row r="65" spans="1:6">
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>36.9</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="2"/>
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1825</v>
       </c>
@@ -7823,8 +8823,20 @@
       <c r="F65">
         <v>13.475645198133495</v>
       </c>
-    </row>
-    <row r="66" spans="1:6">
+      <c r="H65">
+        <f t="shared" si="0"/>
+        <v>33.4</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="2"/>
+        <v>32.700000000000003</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1855</v>
       </c>
@@ -7834,17 +8846,8 @@
       <c r="C66">
         <v>500</v>
       </c>
-      <c r="D66">
-        <v>316</v>
-      </c>
-      <c r="E66">
-        <v>-37.756959123975086</v>
-      </c>
-      <c r="F66">
-        <v>39.435644885762571</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1885</v>
       </c>
@@ -7854,17 +8857,8 @@
       <c r="C67">
         <v>500</v>
       </c>
-      <c r="D67">
-        <v>305</v>
-      </c>
-      <c r="E67">
-        <v>-1.0033046144804771</v>
-      </c>
-      <c r="F67">
-        <v>1.8707464851816269</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1915</v>
       </c>
@@ -7874,33 +8868,27 @@
       <c r="C68">
         <v>500</v>
       </c>
-      <c r="D68">
-        <v>413</v>
-      </c>
-      <c r="E68">
-        <v>-0.89970008462353257</v>
-      </c>
-      <c r="F68">
-        <v>1.7692950143958737</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -7908,7 +8896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -7916,7 +8904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -7936,7 +8924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>25</v>
       </c>
@@ -7956,7 +8944,7 @@
         <v>1.6360000000050299</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>85</v>
       </c>
@@ -7976,7 +8964,7 @@
         <v>1.6555855941298321</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>145</v>
       </c>
@@ -7996,7 +8984,7 @@
         <v>1.5573828411829087</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>205</v>
       </c>
@@ -8016,7 +9004,7 @@
         <v>2.2928217926927239</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>265</v>
       </c>
@@ -8036,7 +9024,7 @@
         <v>3.0118089124192711</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>325</v>
       </c>
@@ -8056,7 +9044,7 @@
         <v>9.0694278279672247</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>385</v>
       </c>
@@ -8076,7 +9064,7 @@
         <v>13.692264075837642</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>445</v>
       </c>
@@ -8096,7 +9084,7 @@
         <v>7.8401055932837238</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>505</v>
       </c>
@@ -8116,7 +9104,7 @@
         <v>21.357151762468618</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>565</v>
       </c>
@@ -8136,7 +9124,7 @@
         <v>8.4265733947410109</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>625</v>
       </c>
@@ -8156,7 +9144,7 @@
         <v>3.8718564035047844</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>685</v>
       </c>
@@ -8176,7 +9164,7 @@
         <v>2.4741459694163979</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>745</v>
       </c>
@@ -8196,7 +9184,7 @@
         <v>2.1382141464971216</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>805</v>
       </c>
@@ -8216,7 +9204,7 @@
         <v>1.9965330473984777</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>865</v>
       </c>
@@ -8236,7 +9224,7 @@
         <v>2.5861904405884228</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>925</v>
       </c>
@@ -8256,7 +9244,7 @@
         <v>3.3872966376813523</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>985</v>
       </c>
@@ -8276,7 +9264,7 @@
         <v>31.529621895863993</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1045</v>
       </c>
@@ -8296,7 +9284,7 @@
         <v>57.807759157366334</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1105</v>
       </c>
@@ -8316,7 +9304,7 @@
         <v>6.1259702932743636</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1165</v>
       </c>
@@ -8336,7 +9324,7 @@
         <v>8.4873780794326183</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1225</v>
       </c>
@@ -8356,7 +9344,7 @@
         <v>3.2408522349053861</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1285</v>
       </c>

</xml_diff>